<commit_message>
update, separate, add categories
</commit_message>
<xml_diff>
--- a/parser/my_project.xlsx
+++ b/parser/my_project.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kiss\github\gitdev\parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G.Tishchenko\Desktop\myfiles\dev\gitdev\parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A1DD64-0305-42EB-BAC2-FAA02FEBABC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="760" firstSheet="4" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="760" firstSheet="4" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,8 +24,9 @@
     <sheet name="Интерфейс" sheetId="11" r:id="rId10"/>
     <sheet name="Интерфейс (2)" sheetId="13" r:id="rId11"/>
     <sheet name="Интерфейс (QT_Designer)" sheetId="15" r:id="rId12"/>
-    <sheet name="Widgets" sheetId="14" r:id="rId13"/>
-    <sheet name="Список ссылок" sheetId="16" r:id="rId14"/>
+    <sheet name="cmd interface" sheetId="17" r:id="rId13"/>
+    <sheet name="Widgets" sheetId="14" r:id="rId14"/>
+    <sheet name="Список ссылок" sheetId="16" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Интерфейс!$A$17:$C$39</definedName>
@@ -34,7 +34,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Интерфейс (QT_Designer)'!$A$1:$J$76</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Категории!$A$1:$H$12</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="354">
   <si>
     <t>id</t>
   </si>
@@ -1299,13 +1299,64 @@
   <si>
     <t>https://www.citilink.ru/product/kartrider-vneshnii-buro-bu-cr-3101-chernyi-1001427/</t>
   </si>
+  <si>
+    <t>Команда</t>
+  </si>
+  <si>
+    <t>Закрыть программу</t>
+  </si>
+  <si>
+    <t>Вывести все экземпляры</t>
+  </si>
+  <si>
+    <t>Добавление экземпляров</t>
+  </si>
+  <si>
+    <t>2,1</t>
+  </si>
+  <si>
+    <t>2,2</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>2,0</t>
+  </si>
+  <si>
+    <t>2,00</t>
+  </si>
+  <si>
+    <t>Назад</t>
+  </si>
+  <si>
+    <t>Добавить предмет</t>
+  </si>
+  <si>
+    <t>Добавить модель</t>
+  </si>
+  <si>
+    <t>Описание</t>
+  </si>
+  <si>
+    <t>3,1</t>
+  </si>
+  <si>
+    <t>3,2</t>
+  </si>
+  <si>
+    <t>Выбор предмета</t>
+  </si>
+  <si>
+    <t>Выбор модели</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -1691,9 +1742,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1752,13 +1803,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1919,6 +1970,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2013,23 +2065,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2065,23 +2100,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -2257,7 +2275,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE58"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -3417,7 +3435,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4149,7 +4167,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K76"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -5920,18 +5938,18 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J76" xr:uid="{00000000-0009-0000-0000-00000A000000}"/>
+  <autoFilter ref="A1:J76"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -7699,7 +7717,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J76" xr:uid="{00000000-0009-0000-0000-00000B000000}">
+  <autoFilter ref="A1:J76">
     <filterColumn colId="3">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -7712,7 +7730,167 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="103" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="103" t="s">
+        <v>201</v>
+      </c>
+      <c r="B3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="103" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" t="s">
+        <v>340</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="103" t="s">
+        <v>341</v>
+      </c>
+      <c r="B5" t="s">
+        <v>347</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="103" t="s">
+        <v>342</v>
+      </c>
+      <c r="B6" t="s">
+        <v>348</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="103" t="s">
+        <v>344</v>
+      </c>
+      <c r="B7" t="s">
+        <v>346</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="103" t="s">
+        <v>345</v>
+      </c>
+      <c r="B8" t="s">
+        <v>338</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="103" t="s">
+        <v>206</v>
+      </c>
+      <c r="B9" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="103" t="s">
+        <v>350</v>
+      </c>
+      <c r="B10" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="103" t="s">
+        <v>351</v>
+      </c>
+      <c r="B11" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="103"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="103" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="103" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="103" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="103" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="103" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="103" t="s">
+        <v>203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A8:U54"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -8316,7 +8494,7 @@
       <c r="M43" s="54"/>
       <c r="N43" s="54"/>
     </row>
-    <row r="44" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="39" x14ac:dyDescent="0.25">
       <c r="A44" s="54"/>
       <c r="B44" s="54"/>
       <c r="C44" s="54"/>
@@ -8510,8 +8688,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8554,7 +8732,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8968,7 +9146,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9112,7 +9290,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9458,14 +9636,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H12" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
+  <autoFilter ref="A1:H12"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9514,7 +9692,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9528,7 +9706,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9560,7 +9738,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9574,7 +9752,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>